<commit_message>
remove treatment column from evap sheet
</commit_message>
<xml_diff>
--- a/data-raw/fluxes/lf_05-bay/lf_05-bay_d_2020-01-24.xlsx
+++ b/data-raw/fluxes/lf_05-bay/lf_05-bay_d_2020-01-24.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Documents/data_working/data_packages/hypoxia.flux.analysis.1/inst/extdata/fluxes/lf_05-bay/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Dropbox (Partners HealthCare)/Copeland.2021.hypoxia.flux/data-raw/fluxes/lf_05-bay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B8DF44-FD16-B740-B8DF-CB5B6E56E272}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10072C8-CAFE-E74D-A899-BC4D2FD0BFD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15280" yWindow="2040" windowWidth="29060" windowHeight="16940" xr2:uid="{101A82DF-E6B5-5B46-9986-3500AB660F6E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="11">
   <si>
     <t>time</t>
   </si>
@@ -62,9 +62,6 @@
     <t>run</t>
   </si>
   <si>
-    <t>treatment</t>
-  </si>
-  <si>
     <t>oxygen</t>
   </si>
   <si>
@@ -73,15 +70,12 @@
   <si>
     <t>0.5%</t>
   </si>
-  <si>
-    <t>DMSO</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -110,10 +104,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
@@ -430,168 +423,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7685FC2E-8A1C-C645-8D24-132AF64BA898}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B11"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="2" max="2" width="10.83203125" style="2"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B2">
+        <v>-24</v>
+      </c>
+      <c r="C2">
+        <v>57.676000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
+      <c r="C3">
+        <v>69.417000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>24</v>
+      </c>
+      <c r="C4">
+        <v>69.174000000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>48</v>
+      </c>
+      <c r="C5">
+        <v>68.927999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>72</v>
+      </c>
+      <c r="C6">
+        <v>68.662000000000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2">
+      <c r="B7">
         <v>-24</v>
       </c>
-      <c r="D2">
-        <v>57.676000000000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="3" t="s">
+      <c r="C7">
+        <v>58.292999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3">
+      <c r="B8">
         <v>0</v>
       </c>
-      <c r="D3">
-        <v>69.417000000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="3" t="s">
+      <c r="C8">
+        <v>70.126000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4">
+      <c r="B9">
         <v>24</v>
       </c>
-      <c r="D4">
-        <v>69.174000000000007</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="3" t="s">
+      <c r="C9">
+        <v>69.843000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5">
+      <c r="B10">
         <v>48</v>
       </c>
-      <c r="D5">
-        <v>68.927999999999997</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="3" t="s">
+      <c r="C10">
+        <v>69.538000000000011</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6">
+      <c r="B11">
         <v>72</v>
       </c>
-      <c r="D6">
-        <v>68.662000000000006</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7">
-        <v>-24</v>
-      </c>
-      <c r="D7">
-        <v>58.292999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>70.126000000000005</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9">
-        <v>24</v>
-      </c>
-      <c r="D9">
-        <v>69.843000000000004</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10">
-        <v>48</v>
-      </c>
-      <c r="D10">
-        <v>69.538000000000011</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C11">
-        <v>72</v>
-      </c>
-      <c r="D11">
         <v>69.211000000000013</v>
       </c>
     </row>
@@ -606,9 +563,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -628,7 +585,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -645,7 +602,7 @@
         <v>9.6210000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -663,7 +620,7 @@
         <v>63.939</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -681,7 +638,7 @@
         <v>118.887</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -699,7 +656,7 @@
         <v>204.29400000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -717,7 +674,7 @@
         <v>403.45600000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -735,7 +692,7 @@
         <v>736.01599999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -753,7 +710,7 @@
         <v>1428.027</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -770,7 +727,7 @@
         <v>2781.386</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -787,7 +744,7 @@
         <v>171.06899999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -805,7 +762,7 @@
         <v>155.66900000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -823,7 +780,7 @@
         <v>208.45</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -841,7 +798,7 @@
         <v>370.202</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -859,7 +816,7 @@
         <v>537.28700000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -877,7 +834,7 @@
         <v>515.01400000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -895,7 +852,7 @@
         <v>1092.143</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -913,7 +870,7 @@
         <v>670.14099999999996</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -931,7 +888,7 @@
         <v>907.36800000000005</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -949,7 +906,7 @@
         <v>1743.452</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -967,7 +924,7 @@
         <v>1397.579</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -985,7 +942,7 @@
         <v>1705.1679999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1003,7 +960,7 @@
         <v>162.56200000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1021,7 +978,7 @@
         <v>199.58</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -1039,7 +996,7 @@
         <v>261.13499999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -1057,7 +1014,7 @@
         <v>265.202</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1075,7 +1032,7 @@
         <v>443.84199999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -1093,7 +1050,7 @@
         <v>340.99799999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -1111,7 +1068,7 @@
         <v>571.47299999999996</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1129,7 +1086,7 @@
         <v>781.84500000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -1147,7 +1104,7 @@
         <v>604.14599999999996</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -1165,7 +1122,7 @@
         <v>742.70299999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -1183,7 +1140,7 @@
         <v>873.101</v>
       </c>
     </row>
-    <row r="33" spans="1:35">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1201,7 +1158,7 @@
         <v>514.947</v>
       </c>
     </row>
-    <row r="34" spans="1:35">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -1218,7 +1175,7 @@
         <v>10.451000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:35">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -1237,7 +1194,7 @@
       </c>
       <c r="AI35" s="1"/>
     </row>
-    <row r="36" spans="1:35">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -1256,7 +1213,7 @@
       </c>
       <c r="AI36" s="1"/>
     </row>
-    <row r="37" spans="1:35">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -1275,7 +1232,7 @@
       </c>
       <c r="AI37" s="1"/>
     </row>
-    <row r="38" spans="1:35">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -1293,7 +1250,7 @@
         <v>382.26100000000002</v>
       </c>
     </row>
-    <row r="39" spans="1:35">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -1311,7 +1268,7 @@
         <v>754.79700000000003</v>
       </c>
     </row>
-    <row r="40" spans="1:35">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -1329,7 +1286,7 @@
         <v>1368.845</v>
       </c>
     </row>
-    <row r="41" spans="1:35">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -1346,7 +1303,7 @@
         <v>2802.2739999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:35">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -1363,7 +1320,7 @@
         <v>732.10699999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:35">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -1381,7 +1338,7 @@
         <v>161.92599999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:35">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -1399,7 +1356,7 @@
         <v>163.453</v>
       </c>
     </row>
-    <row r="45" spans="1:35">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>5</v>
       </c>
@@ -1417,7 +1374,7 @@
         <v>318.43200000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:35">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>5</v>
       </c>
@@ -1435,7 +1392,7 @@
         <v>307.88900000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:35">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -1453,7 +1410,7 @@
         <v>253.94499999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:35">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>5</v>
       </c>
@@ -1471,7 +1428,7 @@
         <v>466.93400000000003</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -1489,7 +1446,7 @@
         <v>425.00799999999998</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -1507,7 +1464,7 @@
         <v>496.64499999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -1525,7 +1482,7 @@
         <v>702.09299999999996</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -1543,7 +1500,7 @@
         <v>637.19399999999996</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>5</v>
       </c>
@@ -1561,7 +1518,7 @@
         <v>516.70699999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>5</v>
       </c>
@@ -1579,7 +1536,7 @@
         <v>162.626</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>5</v>
       </c>
@@ -1597,7 +1554,7 @@
         <v>164.34800000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>5</v>
       </c>
@@ -1615,7 +1572,7 @@
         <v>198.857</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>5</v>
       </c>
@@ -1633,7 +1590,7 @@
         <v>252.393</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>5</v>
       </c>
@@ -1651,7 +1608,7 @@
         <v>344.214</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>5</v>
       </c>
@@ -1669,7 +1626,7 @@
         <v>271.29300000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>5</v>
       </c>
@@ -1687,7 +1644,7 @@
         <v>482.22500000000002</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>5</v>
       </c>
@@ -1705,7 +1662,7 @@
         <v>519.28200000000004</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>5</v>
       </c>
@@ -1723,7 +1680,7 @@
         <v>564.68200000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>5</v>
       </c>
@@ -1741,7 +1698,7 @@
         <v>691.87599999999998</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>5</v>
       </c>
@@ -1759,7 +1716,7 @@
         <v>572.86199999999997</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>5</v>
       </c>
@@ -1788,9 +1745,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1810,7 +1767,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1821,7 +1778,7 @@
         <v>4.3900000000000002E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1832,7 +1789,7 @@
         <v>0.17560000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1843,7 +1800,7 @@
         <v>0.3291</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1854,7 +1811,7 @@
         <v>0.4531</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1865,7 +1822,7 @@
         <v>0.62790000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1876,7 +1833,7 @@
         <v>0.86709999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1887,7 +1844,7 @@
         <v>1.1336999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1898,7 +1855,7 @@
         <v>1.4449000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1909,7 +1866,7 @@
         <v>0.84350000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1921,7 +1878,7 @@
         <v>0.83950000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1933,7 +1890,7 @@
         <v>0.85129999999999995</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1945,7 +1902,7 @@
         <v>0.80520000000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1957,7 +1914,7 @@
         <v>0.80310000000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1969,7 +1926,7 @@
         <v>0.84199999999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1981,7 +1938,7 @@
         <v>0.81299999999999994</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1993,7 +1950,7 @@
         <v>0.74519999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -2005,7 +1962,7 @@
         <v>0.78969999999999996</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -2017,7 +1974,7 @@
         <v>0.75870000000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -2029,7 +1986,7 @@
         <v>0.71150000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -2041,7 +1998,7 @@
         <v>0.63570000000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -2053,7 +2010,7 @@
         <v>0.79369999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -2065,7 +2022,7 @@
         <v>0.80589999999999995</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -2077,7 +2034,7 @@
         <v>0.86029999999999995</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -2089,7 +2046,7 @@
         <v>0.7944</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -2101,7 +2058,7 @@
         <v>0.78100000000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -2113,7 +2070,7 @@
         <v>0.83830000000000005</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -2125,7 +2082,7 @@
         <v>0.76790000000000003</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -2137,7 +2094,7 @@
         <v>0.79320000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -2149,7 +2106,7 @@
         <v>0.77029999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -2161,7 +2118,7 @@
         <v>0.77049999999999996</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -2173,7 +2130,7 @@
         <v>0.70189999999999997</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -2185,7 +2142,7 @@
         <v>0.78390000000000004</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -2197,7 +2154,7 @@
         <v>0.84850000000000003</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -2209,7 +2166,7 @@
         <v>0.79120000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -2221,7 +2178,7 @@
         <v>0.8175</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -2233,7 +2190,7 @@
         <v>0.88339999999999996</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -2245,7 +2202,7 @@
         <v>0.81010000000000004</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -2257,7 +2214,7 @@
         <v>0.83030000000000004</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -2269,7 +2226,7 @@
         <v>0.82389999999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -2281,7 +2238,7 @@
         <v>0.78790000000000004</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -2293,7 +2250,7 @@
         <v>0.8236</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -2305,7 +2262,7 @@
         <v>0.8639</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -2317,7 +2274,7 @@
         <v>0.78659999999999997</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -2329,7 +2286,7 @@
         <v>0.85309999999999997</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -2341,7 +2298,7 @@
         <v>0.84730000000000005</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -2353,7 +2310,7 @@
         <v>0.78239999999999998</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>4</v>
       </c>
@@ -2365,7 +2322,7 @@
         <v>0.80420000000000003</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -2377,7 +2334,7 @@
         <v>0.85880000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -2389,7 +2346,7 @@
         <v>0.83379999999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -2401,7 +2358,7 @@
         <v>0.85209999999999997</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>4</v>
       </c>
@@ -2413,7 +2370,7 @@
         <v>0.8407</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>4</v>
       </c>
@@ -2425,7 +2382,7 @@
         <v>0.81969999999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>4</v>
       </c>
@@ -2437,7 +2394,7 @@
         <v>0.85129999999999995</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>4</v>
       </c>
@@ -2449,7 +2406,7 @@
         <v>0.81200000000000006</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>4</v>
       </c>
@@ -2461,7 +2418,7 @@
         <v>0.82709999999999995</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>4</v>
       </c>
@@ -2484,9 +2441,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -2506,7 +2463,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2517,7 +2474,7 @@
         <v>2128.5830000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2528,7 +2485,7 @@
         <v>2591.0610000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2539,7 +2496,7 @@
         <v>3687.625</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2550,7 +2507,7 @@
         <v>5191.7169999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2561,7 +2518,7 @@
         <v>10035.664000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -2572,7 +2529,7 @@
         <v>19860.506000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -2583,7 +2540,7 @@
         <v>29742.594000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2591,7 +2548,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -2602,7 +2559,7 @@
         <v>2940.8739999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -2614,7 +2571,7 @@
         <v>3021.6689999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -2626,7 +2583,7 @@
         <v>3038.884</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -2638,7 +2595,7 @@
         <v>5288.6030000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -2650,7 +2607,7 @@
         <v>4868.3739999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -2662,7 +2619,7 @@
         <v>4842.3019999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -2674,7 +2631,7 @@
         <v>10263.932000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -2683,7 +2640,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -2695,7 +2652,7 @@
         <v>10040.829</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -2707,7 +2664,7 @@
         <v>20334.153999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -2719,7 +2676,7 @@
         <v>17833.844000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -2731,7 +2688,7 @@
         <v>17757.192999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -2743,7 +2700,7 @@
         <v>2933.8330000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -2755,7 +2712,7 @@
         <v>2993.8519999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -2767,7 +2724,7 @@
         <v>2775.7330000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -2776,7 +2733,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -2788,7 +2745,7 @@
         <v>5863.2060000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -2800,7 +2757,7 @@
         <v>5270.4340000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -2812,7 +2769,7 @@
         <v>11318.012000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -2824,7 +2781,7 @@
         <v>10362.806</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -2836,7 +2793,7 @@
         <v>10392.415000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -2848,7 +2805,7 @@
         <v>20911.143</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -2860,7 +2817,7 @@
         <v>19813.287</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -2869,7 +2826,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -2881,7 +2838,7 @@
         <v>2997.1329999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -2893,7 +2850,7 @@
         <v>3008.2080000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -2905,7 +2862,7 @@
         <v>2969.1109999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -2917,7 +2874,7 @@
         <v>4450.8980000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -2929,7 +2886,7 @@
         <v>4426.8670000000002</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -2941,7 +2898,7 @@
         <v>4253.74</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -2953,7 +2910,7 @@
         <v>7767.4790000000003</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -2962,7 +2919,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -2974,7 +2931,7 @@
         <v>7023.47</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -2986,7 +2943,7 @@
         <v>11081.501</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -2998,7 +2955,7 @@
         <v>9886.5920000000006</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -3010,7 +2967,7 @@
         <v>9291.8760000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -3022,7 +2979,7 @@
         <v>2975.6410000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -3034,7 +2991,7 @@
         <v>2994.556</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>4</v>
       </c>
@@ -3046,7 +3003,7 @@
         <v>3106.0650000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -3058,7 +3015,7 @@
         <v>4649.5050000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -3070,7 +3027,7 @@
         <v>4329.9790000000003</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -3082,7 +3039,7 @@
         <v>4170.268</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>4</v>
       </c>
@@ -3094,7 +3051,7 @@
         <v>7445.55</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>4</v>
       </c>
@@ -3106,7 +3063,7 @@
         <v>7051.1090000000004</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>4</v>
       </c>
@@ -3118,7 +3075,7 @@
         <v>7024.47</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>4</v>
       </c>
@@ -3130,7 +3087,7 @@
         <v>12300.977999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>4</v>
       </c>
@@ -3142,7 +3099,7 @@
         <v>9743.7929999999997</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>4</v>
       </c>

</xml_diff>